<commit_message>
add: detailled role content
</commit_message>
<xml_diff>
--- a/projects.xlsx
+++ b/projects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ismai\game-design-portfolio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ismai\Documents\Taf\Portfolio\mon-portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D23AE4-3BE9-4D5D-9F22-DD95B55F5116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBD3FC1-6C3B-4033-89CF-B5B4D4B13236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="4" xr2:uid="{F9D69F46-245A-4807-AB9A-128EFEE84FB3}"/>
+    <workbookView xWindow="38280" yWindow="-5640" windowWidth="16440" windowHeight="28320" activeTab="4" xr2:uid="{F9D69F46-245A-4807-AB9A-128EFEE84FB3}"/>
   </bookViews>
   <sheets>
     <sheet name="BLCS" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="96">
   <si>
     <t>Missing Media</t>
   </si>
@@ -104,9 +104,6 @@
     <t>Lava chase situation (lava_chase_situation.gif)</t>
   </si>
   <si>
-    <t>Final fall sequence (final_fall.gif)</t>
-  </si>
-  <si>
     <t>Destructible walls in action (destructible_walls.gif)</t>
   </si>
   <si>
@@ -122,9 +119,6 @@
     <t>Gamefeel research document (research_document.png)</t>
   </si>
   <si>
-    <t>Ball bouncing with squash-stretch (ball_bouncing.gif)</t>
-  </si>
-  <si>
     <t>Ball in flame at high velocity (ball_in_flame.gif)</t>
   </si>
   <si>
@@ -140,9 +134,6 @@
     <t>Credits sequence playable (credits_sequence.mp4)</t>
   </si>
   <si>
-    <t>Visual novel gameplay screenshot (gameplay_screenshot.png)</t>
-  </si>
-  <si>
     <t>Miro branching tree diagram (branching_tree.png)</t>
   </si>
   <si>
@@ -336,6 +327,9 @@
   </si>
   <si>
     <t>☐</t>
+  </si>
+  <si>
+    <t>Visual novel gameplay video youtube</t>
   </si>
 </sst>
 </file>
@@ -365,12 +359,30 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -385,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -397,6 +409,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -734,16 +749,16 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A5" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="60.578125" customWidth="1"/>
-    <col min="2" max="2" width="8.578125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="60.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -751,45 +766,45 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -808,16 +823,16 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="60.578125" customWidth="1"/>
-    <col min="2" max="2" width="8.578125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="60.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -825,85 +840,85 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
+    <row r="2" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -922,16 +937,16 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="60.578125" customWidth="1"/>
-    <col min="2" max="2" width="8.578125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="60.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -939,139 +954,123 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B19" s="2">
-        <f>COUNTIF(B2:B16,"☐")</f>
-        <v>15</v>
+        <f>COUNTIF(B2:B14,"☐")</f>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1084,16 +1083,16 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="60.578125" customWidth="1"/>
-    <col min="2" max="2" width="8.578125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="60.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1101,61 +1100,61 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A3" t="s">
+      <c r="B5" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A4" t="s">
+      <c r="B6" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A7" t="s">
-        <v>37</v>
-      </c>
       <c r="B7" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -1173,17 +1172,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79AAE71A-C4F1-4AA1-960B-5293CFCE8E9F}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="60.578125" customWidth="1"/>
-    <col min="2" max="2" width="8.578125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="60.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1191,269 +1190,269 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
+    <row r="2" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A3" t="s">
+      <c r="B5" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A4" t="s">
+      <c r="B6" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A5" t="s">
+      <c r="B7" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A6" t="s">
+      <c r="B8" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A7" t="s">
+      <c r="B9" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A8" t="s">
+      <c r="B10" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A9" t="s">
+      <c r="B11" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A10" t="s">
+      <c r="B12" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A11" t="s">
+      <c r="B13" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A12" t="s">
+      <c r="B14" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A13" t="s">
+      <c r="B15" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A14" t="s">
+      <c r="B16" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A15" t="s">
+      <c r="B17" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A16" t="s">
+      <c r="B18" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A17" t="s">
+      <c r="B19" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A18" t="s">
+      <c r="B20" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A19" t="s">
+      <c r="B21" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A20" t="s">
+      <c r="B22" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A21" t="s">
+      <c r="B23" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A22" t="s">
+      <c r="B24" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A23" t="s">
+      <c r="B25" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A24" t="s">
+      <c r="B26" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A25" t="s">
+      <c r="B27" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A26" t="s">
+      <c r="B28" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>62</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A27" t="s">
+      <c r="B29" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>63</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A28" t="s">
+      <c r="B30" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A29" t="s">
+      <c r="B31" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A30" t="s">
+      <c r="B32" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A31" t="s">
-        <v>67</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A32" t="s">
-        <v>68</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A33" t="s">
-        <v>69</v>
-      </c>
       <c r="B33" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B35" s="2"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
@@ -1473,16 +1472,16 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A8" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="60.578125" customWidth="1"/>
-    <col min="2" max="2" width="8.578125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="60.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1490,69 +1489,69 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A3" t="s">
+      <c r="B5" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A4" t="s">
+      <c r="B6" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A5" t="s">
+      <c r="B7" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A8" t="s">
-        <v>76</v>
-      </c>
       <c r="B8" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -1571,16 +1570,16 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B21"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="60.578125" customWidth="1"/>
-    <col min="2" max="2" width="8.578125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="60.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1588,173 +1587,173 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A3" t="s">
+      <c r="B5" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A4" t="s">
+      <c r="B6" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A5" t="s">
+      <c r="B7" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A6" t="s">
+      <c r="B8" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A7" t="s">
+      <c r="B9" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A8" t="s">
+      <c r="B10" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>83</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A9" t="s">
+      <c r="B11" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A10" t="s">
+      <c r="B12" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>85</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A11" t="s">
+      <c r="B13" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A12" t="s">
+      <c r="B14" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>87</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A13" t="s">
+      <c r="B15" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A14" t="s">
+      <c r="B16" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>89</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A15" t="s">
+      <c r="B17" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>90</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A16" t="s">
+      <c r="B18" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A17" t="s">
+      <c r="B19" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A18" t="s">
+      <c r="B20" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A19" t="s">
-        <v>94</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A20" t="s">
-        <v>95</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="19.8" x14ac:dyDescent="0.8">
-      <c r="A21" t="s">
-        <v>96</v>
-      </c>
       <c r="B21" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
add: finish detailled content
</commit_message>
<xml_diff>
--- a/projects.xlsx
+++ b/projects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ismai\Documents\Taf\Portfolio\mon-portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBD3FC1-6C3B-4033-89CF-B5B4D4B13236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC67455-25C6-4691-B0A1-EE57EEB30B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-5640" windowWidth="16440" windowHeight="28320" activeTab="4" xr2:uid="{F9D69F46-245A-4807-AB9A-128EFEE84FB3}"/>
+    <workbookView xWindow="38280" yWindow="-5640" windowWidth="16440" windowHeight="28320" firstSheet="2" activeTab="2" xr2:uid="{F9D69F46-245A-4807-AB9A-128EFEE84FB3}"/>
   </bookViews>
   <sheets>
     <sheet name="BLCS" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="93">
   <si>
     <t>Missing Media</t>
   </si>
@@ -161,9 +161,6 @@
     <t>Inspector view of audio system (inspector.png)</t>
   </si>
   <si>
-    <t>Combat HUD - threat tracking #1 (hud1.png)</t>
-  </si>
-  <si>
     <t>Combat HUD - threat tracking #2 (hud2.png)</t>
   </si>
   <si>
@@ -179,9 +176,6 @@
     <t>Hub progression - before/after (hubprogression.png)</t>
   </si>
   <si>
-    <t>Hub path to action (hubpath.png)</t>
-  </si>
-  <si>
     <t>Mission briefing corridor (corridor.png)</t>
   </si>
   <si>
@@ -240,9 +234,6 @@
   </si>
   <si>
     <t>Moodboard - visual direction (moodboardvis.png)</t>
-  </si>
-  <si>
-    <t>PowerPoint commentary view (pwpcommentary.png)</t>
   </si>
   <si>
     <t>Health bar with spinning vinyl (health_vinyl.gif)</t>
@@ -359,7 +350,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -384,6 +375,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -397,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -412,6 +409,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -771,7 +769,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
@@ -779,7 +777,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
@@ -787,7 +785,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
@@ -795,7 +793,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -823,7 +821,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,67 +839,67 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="A9" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
@@ -909,7 +907,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -936,7 +934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8C7ADD9-314C-4529-9D5A-D65F15A65061}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -959,7 +957,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
@@ -967,7 +965,7 @@
         <v>18</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
@@ -975,7 +973,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
@@ -983,7 +981,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
@@ -991,7 +989,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
@@ -999,7 +997,7 @@
         <v>22</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
@@ -1007,7 +1005,7 @@
         <v>23</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
@@ -1015,7 +1013,7 @@
         <v>24</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
@@ -1023,7 +1021,7 @@
         <v>25</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
@@ -1031,7 +1029,7 @@
         <v>26</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
@@ -1039,7 +1037,7 @@
         <v>27</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
@@ -1047,7 +1045,7 @@
         <v>28</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
@@ -1055,7 +1053,7 @@
         <v>29</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1081,6 +1079,476 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19D0BE3A-5BF3-4045-B9A7-2A6A3C00A2AF}">
   <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="60.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2">
+        <f>COUNTIF(B2:B7,"☐")</f>
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79AAE71A-C4F1-4AA1-960B-5293CFCE8E9F}">
+  <dimension ref="A1:B36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="60.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A13" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A16" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A17" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A18" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A19" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A20" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A21" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A22" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A23" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A24" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A25" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A26" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A27" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="B33" s="3"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="2">
+        <f>COUNTIF(B2:B33,"☐")</f>
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8108A42-6D65-4BA4-A5A7-96DEC7485C00}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="60.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2">
+        <f>COUNTIF(B2:B8,"☐")</f>
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28BF2AB3-CA56-4193-85C0-44290F3DD3BB}">
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
@@ -1101,650 +1569,163 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
-        <v>95</v>
+      <c r="A2" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>30</v>
+      <c r="A3" s="8" t="s">
+        <v>72</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>31</v>
+      <c r="A4" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>32</v>
+      <c r="A5" s="8" t="s">
+        <v>74</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
-        <v>33</v>
+      <c r="A6" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
-        <v>34</v>
+      <c r="A7" s="8" t="s">
+        <v>76</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="2">
-        <f>COUNTIF(B2:B7,"☐")</f>
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79AAE71A-C4F1-4AA1-960B-5293CFCE8E9F}">
-  <dimension ref="A1:B36"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="60.5703125" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" style="4" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>41</v>
+      <c r="A8" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>42</v>
+      <c r="A9" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>43</v>
+      <c r="A10" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>44</v>
+      <c r="A11" s="8" t="s">
+        <v>80</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>45</v>
+      <c r="A12" s="8" t="s">
+        <v>81</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>46</v>
+      <c r="A13" s="8" t="s">
+        <v>82</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>47</v>
+      <c r="A14" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>48</v>
+      <c r="A15" s="8" t="s">
+        <v>84</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>49</v>
+      <c r="A16" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>50</v>
+      <c r="A17" s="8" t="s">
+        <v>86</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>51</v>
+      <c r="A18" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>56</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>57</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>58</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>59</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>60</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>61</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>62</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>63</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>64</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>65</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>66</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="2"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B36" s="2">
-        <f>COUNTIF(B2:B33,"☐")</f>
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8108A42-6D65-4BA4-A5A7-96DEC7485C00}">
-  <dimension ref="A1:B11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A2:A8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="60.5703125" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" style="4" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="2">
-        <f>COUNTIF(B2:B8,"☐")</f>
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28BF2AB3-CA56-4193-85C0-44290F3DD3BB}">
-  <dimension ref="A1:B24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="60.5703125" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" style="4" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>82</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>85</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>87</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A16" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>89</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>90</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="20.25" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>